<commit_message>
social cost of carbon
</commit_message>
<xml_diff>
--- a/IPCC_Carbon_Calculations.xlsx
+++ b/IPCC_Carbon_Calculations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uillinoisedu-my.sharepoint.com/personal/cmptrsn2_illinois_edu/Documents/Ch1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uillinoisedu-my.sharepoint.com/personal/cmptrsn2_illinois_edu/Documents/Chapter2/Floodplain-Experiment-Repo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="687" documentId="8_{81C5A17B-0AA7-4E1F-9EEB-1F73114DAE67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00B3CBB3-0C46-4F10-A41E-06B59E8E7ACD}"/>
+  <xr:revisionPtr revIDLastSave="949" documentId="8_{81C5A17B-0AA7-4E1F-9EEB-1F73114DAE67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{43B212A6-596B-4800-AA6A-999BCFCD0375}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="16155" yWindow="6825" windowWidth="12150" windowHeight="20955" activeTab="1" xr2:uid="{2C906CBC-631A-4B26-833B-3AA2F3C7757D}"/>
+    <workbookView xWindow="16080" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{2C906CBC-631A-4B26-833B-3AA2F3C7757D}"/>
   </bookViews>
   <sheets>
     <sheet name="Joslin estimates" sheetId="1" r:id="rId1"/>
@@ -602,20 +602,20 @@
       <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.85546875" customWidth="1"/>
+    <col min="1" max="1" width="29.88671875" customWidth="1"/>
     <col min="2" max="2" width="29" customWidth="1"/>
-    <col min="3" max="3" width="41.5703125" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" customWidth="1"/>
+    <col min="3" max="3" width="41.5546875" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" customWidth="1"/>
+    <col min="5" max="5" width="12.5546875" customWidth="1"/>
     <col min="6" max="6" width="10" customWidth="1"/>
-    <col min="7" max="7" width="8.28515625" customWidth="1"/>
-    <col min="8" max="8" width="24.28515625" customWidth="1"/>
+    <col min="7" max="7" width="8.33203125" customWidth="1"/>
+    <col min="8" max="8" width="24.33203125" customWidth="1"/>
     <col min="12" max="12" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -641,7 +641,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -669,7 +669,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
@@ -695,7 +695,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
         <v>8</v>
       </c>
@@ -709,7 +709,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
         <v>35</v>
       </c>
@@ -728,12 +728,12 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C6" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
         <v>45</v>
       </c>
@@ -753,7 +753,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
         <v>38</v>
       </c>
@@ -764,7 +764,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
         <v>50</v>
       </c>
@@ -772,7 +772,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
         <v>51</v>
       </c>
@@ -781,7 +781,7 @@
         <v>34.700000000000003</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
         <v>48</v>
       </c>
@@ -798,7 +798,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C12" t="s">
         <v>47</v>
       </c>
@@ -809,7 +809,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C13" t="s">
         <v>52</v>
       </c>
@@ -826,7 +826,7 @@
         <v>0.35602200000000006</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C14" t="s">
         <v>39</v>
       </c>
@@ -843,7 +843,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C15" t="s">
         <v>40</v>
       </c>
@@ -860,7 +860,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C16" t="s">
         <v>25</v>
       </c>
@@ -874,7 +874,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C17" t="s">
         <v>41</v>
       </c>
@@ -891,7 +891,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C18" t="s">
         <v>55</v>
       </c>
@@ -905,7 +905,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>1</v>
       </c>
@@ -925,7 +925,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>2</v>
       </c>
@@ -945,7 +945,7 @@
         <v>75.55680000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>36</v>
       </c>
@@ -962,7 +962,7 @@
         <v>87.12</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>0</v>
       </c>
@@ -979,7 +979,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -999,7 +999,7 @@
         <v>14.879999999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>18</v>
       </c>
@@ -1016,7 +1016,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>17</v>
       </c>
@@ -1036,7 +1036,7 @@
         <v>8.5445280000000015</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>21</v>
       </c>
@@ -1053,7 +1053,7 @@
         <v>17.801100000000002</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>24</v>
       </c>
@@ -1073,7 +1073,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>23</v>
       </c>
@@ -1090,7 +1090,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>53</v>
       </c>
@@ -1110,7 +1110,7 @@
         <v>205.54452800000001</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>34</v>
       </c>
@@ -1127,7 +1127,7 @@
         <v>236.80109999999999</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>54</v>
       </c>
@@ -1147,7 +1147,7 @@
         <v>153.27252800000002</v>
       </c>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>34</v>
       </c>
@@ -1177,17 +1177,17 @@
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.28515625" customWidth="1"/>
-    <col min="2" max="2" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="48.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.33203125" customWidth="1"/>
+    <col min="2" max="2" width="28.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="48.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -1213,7 +1213,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -1241,7 +1241,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>56</v>
       </c>
@@ -1267,7 +1267,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>57</v>
       </c>
@@ -1288,7 +1288,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
         <v>35</v>
       </c>
@@ -1307,12 +1307,12 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C6" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
         <v>45</v>
       </c>
@@ -1332,7 +1332,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
         <v>38</v>
       </c>
@@ -1343,7 +1343,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
         <v>50</v>
       </c>
@@ -1351,7 +1351,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
         <v>51</v>
       </c>
@@ -1360,7 +1360,7 @@
         <v>34.700000000000003</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
         <v>48</v>
       </c>
@@ -1377,7 +1377,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C12" t="s">
         <v>47</v>
       </c>
@@ -1388,7 +1388,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C13" t="s">
         <v>52</v>
       </c>
@@ -1405,7 +1405,7 @@
         <v>0.35602200000000006</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C14" t="s">
         <v>39</v>
       </c>
@@ -1422,7 +1422,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C15" t="s">
         <v>40</v>
       </c>
@@ -1439,7 +1439,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C16" t="s">
         <v>25</v>
       </c>
@@ -1453,7 +1453,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C17" t="s">
         <v>41</v>
       </c>
@@ -1470,7 +1470,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C18" t="s">
         <v>55</v>
       </c>
@@ -1484,7 +1484,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>1</v>
       </c>
@@ -1504,7 +1504,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>2</v>
       </c>
@@ -1524,7 +1524,7 @@
         <v>75.55680000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>36</v>
       </c>
@@ -1541,7 +1541,7 @@
         <v>87.12</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>0</v>
       </c>
@@ -1558,7 +1558,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -1578,7 +1578,7 @@
         <v>10.23</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>18</v>
       </c>
@@ -1595,7 +1595,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>17</v>
       </c>
@@ -1615,7 +1615,7 @@
         <v>5.8743630000000007</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>21</v>
       </c>
@@ -1632,7 +1632,7 @@
         <v>17.801100000000002</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>24</v>
       </c>
@@ -1652,7 +1652,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>23</v>
       </c>
@@ -1669,7 +1669,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>53</v>
       </c>
@@ -1689,7 +1689,7 @@
         <v>198.22436300000001</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>34</v>
       </c>
@@ -1706,7 +1706,7 @@
         <v>236.80109999999999</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>54</v>
       </c>
@@ -1726,7 +1726,7 @@
         <v>145.95236299999999</v>
       </c>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>34</v>
       </c>

</xml_diff>